<commit_message>
created 24to25map and fix for diffsnuxim
- created 24to25map and fix for diffsnuxim
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/24Tto25TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/24Tto25TMap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
-  <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustolopezbao/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46B7CE2A-42D2-4149-AE59-2D36B94FF2BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09B0B323-4DB6-6741-A231-E79B593358C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39380" yWindow="1620" windowWidth="33600" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="33600" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,6 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="952" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="212">
   <si>
     <t>CXCA_SCRN</t>
   </si>
@@ -677,7 +674,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1009,15 +1006,15 @@
   </fills>
   <borders count="12">
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4"/>
@@ -1025,8 +1022,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thick">
         <color theme="4" tint="0.499984740745262"/>
@@ -1034,8 +1031,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.39997558519241921"/>
@@ -1043,12 +1040,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FF7F7F7F"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FF7F7F7F"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FF7F7F7F"/>
       </top>
@@ -1058,12 +1055,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -1073,8 +1070,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -1082,12 +1079,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="double">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
-      </start>
-      <end style="double">
+      </left>
+      <right style="double">
         <color rgb="FF3F3F3F"/>
-      </end>
+      </right>
       <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -1097,12 +1094,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color rgb="FFB2B2B2"/>
-      </end>
+      </right>
       <top style="thin">
         <color rgb="FFB2B2B2"/>
       </top>
@@ -1112,8 +1109,8 @@
       <diagonal/>
     </border>
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1123,12 +1120,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color indexed="64"/>
-      </end>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1138,12 +1135,12 @@
       <diagonal/>
     </border>
     <border>
-      <start style="thin">
+      <left style="thin">
         <color indexed="64"/>
-      </start>
-      <end style="thin">
+      </left>
+      <right style="thin">
         <color indexed="64"/>
-      </end>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1266,7 +1263,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1419,25 +1416,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110%"/>
-                <a:satMod val="105%"/>
-                <a:tint val="67%"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="103%"/>
-                <a:tint val="73%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105%"/>
-                <a:satMod val="109%"/>
-                <a:tint val="81%"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1445,25 +1442,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103%"/>
-                <a:lumMod val="102%"/>
-                <a:tint val="94%"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110%"/>
-                <a:lumMod val="100%"/>
-                <a:shade val="100%"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99%"/>
-                <a:satMod val="120%"/>
-                <a:shade val="78%"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1476,21 +1473,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800%"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -1504,7 +1501,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63%"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1516,32 +1513,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95%"/>
-            <a:satMod val="170%"/>
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93%"/>
-                <a:satMod val="150%"/>
-                <a:shade val="98%"/>
-                <a:lumMod val="102%"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50%">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="98%"/>
-                <a:satMod val="130%"/>
-                <a:shade val="90%"/>
-                <a:lumMod val="103%"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="100%">
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63%"/>
-                <a:satMod val="120%"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -1561,7 +1558,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">

</xml_diff>

<commit_message>
Updated dx uid in 24Tto25TMap to 2024 mer targets
- Updated dx uid to 2024 mer targets and altered cop_year 2023 to reference 24Tto25TMap
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/24Tto25TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/24Tto25TMap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustolopezbao/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09B0B323-4DB6-6741-A231-E79B593358C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2A9F5C-E130-A748-BD37-67353A3B236B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="33600" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2140" yWindow="500" windowWidth="33600" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Map" sheetId="1" r:id="rId1"/>
@@ -599,9 +599,6 @@
     <t>Age/Sex/ProgramStatus;Age/Sex/ProgramStatusCaregiver</t>
   </si>
   <si>
-    <t>DE_GROUP-OuKFZzVk6gr</t>
-  </si>
-  <si>
     <t>2022Oct</t>
   </si>
   <si>
@@ -669,6 +666,9 @@
   </si>
   <si>
     <t>5-14</t>
+  </si>
+  <si>
+    <t>DE_GROUP-TXAVaM4oYMd</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1563,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G20" sqref="G20"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1633,7 +1633,7 @@
         <v>121</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1654,7 +1654,7 @@
         <v>98</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>2</v>
@@ -1677,7 +1677,7 @@
         <v>122</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1698,7 +1698,7 @@
         <v>98</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>2</v>
@@ -1721,7 +1721,7 @@
         <v>123</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -1742,10 +1742,10 @@
         <v>89</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>43</v>
@@ -1765,7 +1765,7 @@
         <v>126</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -1786,10 +1786,10 @@
         <v>119</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>49</v>
@@ -1809,7 +1809,7 @@
         <v>127</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -1830,10 +1830,10 @@
         <v>119</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>49</v>
@@ -1853,7 +1853,7 @@
         <v>128</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -1874,10 +1874,10 @@
         <v>97</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>43</v>
@@ -1897,7 +1897,7 @@
         <v>129</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
@@ -1918,10 +1918,10 @@
         <v>97</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>43</v>
@@ -1941,7 +1941,7 @@
         <v>130</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -1962,7 +1962,7 @@
         <v>94</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>2</v>
@@ -1985,7 +1985,7 @@
         <v>131</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -2006,7 +2006,7 @@
         <v>94</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>2</v>
@@ -2029,7 +2029,7 @@
         <v>132</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
@@ -2050,7 +2050,7 @@
         <v>92</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>2</v>
@@ -2073,7 +2073,7 @@
         <v>133</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -2094,7 +2094,7 @@
         <v>93</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>2</v>
@@ -2117,7 +2117,7 @@
         <v>134</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>9</v>
@@ -2138,7 +2138,7 @@
         <v>96</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>2</v>
@@ -2161,7 +2161,7 @@
         <v>135</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
@@ -2182,7 +2182,7 @@
         <v>92</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>2</v>
@@ -2205,7 +2205,7 @@
         <v>136</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
@@ -2226,7 +2226,7 @@
         <v>95</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>2</v>
@@ -2249,7 +2249,7 @@
         <v>137</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>14</v>
@@ -2270,7 +2270,7 @@
         <v>186</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>185</v>
@@ -2293,7 +2293,7 @@
         <v>177</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>14</v>
@@ -2314,7 +2314,7 @@
         <v>186</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>185</v>
@@ -2337,7 +2337,7 @@
         <v>176</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>14</v>
@@ -2358,10 +2358,10 @@
         <v>181</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>43</v>
@@ -2381,7 +2381,7 @@
         <v>138</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>15</v>
@@ -2402,10 +2402,10 @@
         <v>107</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>49</v>
@@ -2425,7 +2425,7 @@
         <v>139</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>15</v>
@@ -2446,10 +2446,10 @@
         <v>107</v>
       </c>
       <c r="I20" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J20" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>49</v>
@@ -2469,7 +2469,7 @@
         <v>140</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>16</v>
@@ -2490,7 +2490,7 @@
         <v>88</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>47</v>
@@ -2513,7 +2513,7 @@
         <v>141</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>16</v>
@@ -2534,7 +2534,7 @@
         <v>88</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>48</v>
@@ -2557,7 +2557,7 @@
         <v>142</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>18</v>
@@ -2578,10 +2578,10 @@
         <v>89</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>49</v>
@@ -2601,7 +2601,7 @@
         <v>143</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>18</v>
@@ -2622,10 +2622,10 @@
         <v>91</v>
       </c>
       <c r="I24" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J24" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>49</v>
@@ -2645,7 +2645,7 @@
         <v>144</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>18</v>
@@ -2666,10 +2666,10 @@
         <v>91</v>
       </c>
       <c r="I25" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>49</v>
@@ -2689,7 +2689,7 @@
         <v>145</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>18</v>
@@ -2710,10 +2710,10 @@
         <v>91</v>
       </c>
       <c r="I26" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J26" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>49</v>
@@ -2733,7 +2733,7 @@
         <v>146</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>21</v>
@@ -2754,10 +2754,10 @@
         <v>89</v>
       </c>
       <c r="I27" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J27" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>43</v>
@@ -2777,13 +2777,13 @@
         <v>178</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>35</v>
@@ -2798,10 +2798,10 @@
         <v>89</v>
       </c>
       <c r="I28" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J28" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>43</v>
@@ -2821,13 +2821,13 @@
         <v>179</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>35</v>
@@ -2842,7 +2842,7 @@
         <v>92</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>2</v>
@@ -2865,7 +2865,7 @@
         <v>147</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>22</v>
@@ -2886,10 +2886,10 @@
         <v>89</v>
       </c>
       <c r="I30" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J30" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>43</v>
@@ -2909,7 +2909,7 @@
         <v>148</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>22</v>
@@ -2930,7 +2930,7 @@
         <v>92</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>2</v>
@@ -2953,7 +2953,7 @@
         <v>149</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>23</v>
@@ -2974,10 +2974,10 @@
         <v>107</v>
       </c>
       <c r="I32" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J32" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>43</v>
@@ -2997,7 +2997,7 @@
         <v>150</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>23</v>
@@ -3018,10 +3018,10 @@
         <v>107</v>
       </c>
       <c r="I33" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J33" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>43</v>
@@ -3041,7 +3041,7 @@
         <v>151</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>24</v>
@@ -3062,7 +3062,7 @@
         <v>107</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J34" s="6" t="s">
         <v>101</v>
@@ -3085,7 +3085,7 @@
         <v>152</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>24</v>
@@ -3106,7 +3106,7 @@
         <v>107</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>101</v>
@@ -3129,7 +3129,7 @@
         <v>153</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>24</v>
@@ -3150,7 +3150,7 @@
         <v>107</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J36" s="6" t="s">
         <v>101</v>
@@ -3173,7 +3173,7 @@
         <v>154</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>24</v>
@@ -3194,7 +3194,7 @@
         <v>107</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>101</v>
@@ -3217,7 +3217,7 @@
         <v>155</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>25</v>
@@ -3238,10 +3238,10 @@
         <v>89</v>
       </c>
       <c r="I38" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J38" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>43</v>
@@ -3261,7 +3261,7 @@
         <v>156</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>25</v>
@@ -3282,10 +3282,10 @@
         <v>91</v>
       </c>
       <c r="I39" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J39" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>43</v>
@@ -3305,7 +3305,7 @@
         <v>157</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>25</v>
@@ -3326,10 +3326,10 @@
         <v>91</v>
       </c>
       <c r="I40" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J40" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>43</v>
@@ -3349,7 +3349,7 @@
         <v>158</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>25</v>
@@ -3370,10 +3370,10 @@
         <v>91</v>
       </c>
       <c r="I41" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J41" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>43</v>
@@ -3393,7 +3393,7 @@
         <v>159</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>26</v>
@@ -3414,10 +3414,10 @@
         <v>90</v>
       </c>
       <c r="I42" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J42" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>43</v>
@@ -3437,7 +3437,7 @@
         <v>160</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>27</v>
@@ -3458,10 +3458,10 @@
         <v>90</v>
       </c>
       <c r="I43" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J43" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>43</v>
@@ -3481,7 +3481,7 @@
         <v>161</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>27</v>
@@ -3502,7 +3502,7 @@
         <v>93</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>2</v>
@@ -3525,7 +3525,7 @@
         <v>162</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>26</v>
@@ -3546,7 +3546,7 @@
         <v>93</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J45" s="6" t="s">
         <v>2</v>
@@ -3569,7 +3569,7 @@
         <v>163</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>29</v>
@@ -3590,7 +3590,7 @@
         <v>93</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>2</v>
@@ -3613,7 +3613,7 @@
         <v>164</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>29</v>
@@ -3634,7 +3634,7 @@
         <v>93</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J47" s="6" t="s">
         <v>2</v>
@@ -3657,7 +3657,7 @@
         <v>165</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>29</v>
@@ -3678,10 +3678,10 @@
         <v>108</v>
       </c>
       <c r="I48" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J48" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>43</v>
@@ -3701,7 +3701,7 @@
         <v>166</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>29</v>
@@ -3722,10 +3722,10 @@
         <v>108</v>
       </c>
       <c r="I49" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J49" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>43</v>
@@ -3745,7 +3745,7 @@
         <v>167</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>31</v>
@@ -3766,7 +3766,7 @@
         <v>112</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J50" s="6" t="s">
         <v>101</v>
@@ -3789,7 +3789,7 @@
         <v>168</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>31</v>
@@ -3810,7 +3810,7 @@
         <v>112</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J51" s="6" t="s">
         <v>101</v>
@@ -3833,7 +3833,7 @@
         <v>169</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>31</v>
@@ -3854,7 +3854,7 @@
         <v>112</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J52" s="6" t="s">
         <v>101</v>
@@ -3877,7 +3877,7 @@
         <v>170</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>31</v>
@@ -3898,7 +3898,7 @@
         <v>112</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J53" s="6" t="s">
         <v>101</v>
@@ -3921,7 +3921,7 @@
         <v>171</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>33</v>
@@ -3942,10 +3942,10 @@
         <v>90</v>
       </c>
       <c r="I54" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J54" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J54" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>60</v>
@@ -3965,7 +3965,7 @@
         <v>172</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>33</v>
@@ -3986,10 +3986,10 @@
         <v>90</v>
       </c>
       <c r="I55" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J55" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J55" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>60</v>
@@ -4009,7 +4009,7 @@
         <v>173</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>33</v>
@@ -4030,10 +4030,10 @@
         <v>90</v>
       </c>
       <c r="I56" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J56" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J56" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>60</v>
@@ -4053,7 +4053,7 @@
         <v>174</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>0</v>
@@ -4074,10 +4074,10 @@
         <v>90</v>
       </c>
       <c r="I57" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J57" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>49</v>
@@ -4097,7 +4097,7 @@
         <v>180</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>14</v>
@@ -4118,7 +4118,7 @@
         <v>183</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J58" s="6" t="s">
         <v>185</v>
@@ -4138,16 +4138,16 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>35</v>
@@ -4162,10 +4162,10 @@
         <v>89</v>
       </c>
       <c r="I59" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J59" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J59" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>43</v>
@@ -4182,10 +4182,10 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>102</v>
@@ -4200,16 +4200,16 @@
         <v>66</v>
       </c>
       <c r="G60" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H60" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="H60" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="I60" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J60" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>43</v>
@@ -4226,10 +4226,10 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>102</v>
@@ -4244,16 +4244,16 @@
         <v>66</v>
       </c>
       <c r="G61" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="H61" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="H61" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="I61" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J61" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J61" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K61" s="2" t="s">
         <v>43</v>
@@ -4270,10 +4270,10 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>7</v>
@@ -4288,16 +4288,16 @@
         <v>66</v>
       </c>
       <c r="G62" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H62" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="H62" s="3" t="s">
-        <v>210</v>
-      </c>
       <c r="I62" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J62" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J62" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>43</v>
@@ -4314,10 +4314,10 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>7</v>
@@ -4332,16 +4332,16 @@
         <v>66</v>
       </c>
       <c r="G63" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="H63" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="H63" s="3" t="s">
-        <v>210</v>
-      </c>
       <c r="I63" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J63" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J63" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>43</v>
@@ -4358,10 +4358,10 @@
     </row>
     <row r="64" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>7</v>
@@ -4376,16 +4376,16 @@
         <v>66</v>
       </c>
       <c r="G64" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="H64" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="H64" s="7" t="s">
-        <v>206</v>
-      </c>
       <c r="I64" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J64" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J64" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K64" s="2" t="s">
         <v>43</v>
@@ -4402,10 +4402,10 @@
     </row>
     <row r="65" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>7</v>
@@ -4420,16 +4420,16 @@
         <v>66</v>
       </c>
       <c r="G65" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="H65" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="H65" s="7" t="s">
-        <v>206</v>
-      </c>
       <c r="I65" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J65" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J65" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>43</v>
@@ -4446,10 +4446,10 @@
     </row>
     <row r="66" spans="1:14" ht="153" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>5</v>
@@ -4464,16 +4464,16 @@
         <v>66</v>
       </c>
       <c r="G66" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="H66" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="H66" s="8" t="s">
-        <v>208</v>
-      </c>
       <c r="I66" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J66" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J66" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>43</v>
@@ -4493,7 +4493,7 @@
         <v>125</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>7</v>
@@ -4508,16 +4508,16 @@
         <v>66</v>
       </c>
       <c r="G67" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="H67" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="H67" s="7" t="s">
-        <v>204</v>
-      </c>
       <c r="I67" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J67" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J67" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K67" s="2" t="s">
         <v>43</v>
@@ -4537,7 +4537,7 @@
         <v>124</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>7</v>
@@ -4552,16 +4552,16 @@
         <v>66</v>
       </c>
       <c r="G68" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="H68" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="H68" s="7" t="s">
-        <v>204</v>
-      </c>
       <c r="I68" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="J68" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="J68" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="K68" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
updated periods in 24Tto25TMap from 2022Oct to 2023Oct
- updated periods in 24Tto25TMap from 2022Oct to 2023Oct
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/24Tto25TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/24Tto25TMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustolopezbao/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2A9F5C-E130-A748-BD37-67353A3B236B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83EF650-ACA1-4D49-8736-DB3AB8792A55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2140" yWindow="500" windowWidth="33600" windowHeight="20340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -599,9 +599,6 @@
     <t>Age/Sex/ProgramStatus;Age/Sex/ProgramStatusCaregiver</t>
   </si>
   <si>
-    <t>2022Oct</t>
-  </si>
-  <si>
     <t>fy24_age_bands</t>
   </si>
   <si>
@@ -669,6 +666,9 @@
   </si>
   <si>
     <t>DE_GROUP-TXAVaM4oYMd</t>
+  </si>
+  <si>
+    <t>2023Oct</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1563,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1633,7 +1633,7 @@
         <v>121</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1654,7 +1654,7 @@
         <v>98</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>2</v>
@@ -1677,7 +1677,7 @@
         <v>122</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1698,7 +1698,7 @@
         <v>98</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>2</v>
@@ -1721,7 +1721,7 @@
         <v>123</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -1742,10 +1742,10 @@
         <v>89</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J4" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>43</v>
@@ -1765,7 +1765,7 @@
         <v>126</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -1786,10 +1786,10 @@
         <v>119</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J5" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>49</v>
@@ -1809,7 +1809,7 @@
         <v>127</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -1830,10 +1830,10 @@
         <v>119</v>
       </c>
       <c r="I6" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>49</v>
@@ -1853,7 +1853,7 @@
         <v>128</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -1874,10 +1874,10 @@
         <v>97</v>
       </c>
       <c r="I7" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J7" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>43</v>
@@ -1897,7 +1897,7 @@
         <v>129</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
@@ -1918,10 +1918,10 @@
         <v>97</v>
       </c>
       <c r="I8" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>43</v>
@@ -1941,7 +1941,7 @@
         <v>130</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -1962,7 +1962,7 @@
         <v>94</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>2</v>
@@ -1985,7 +1985,7 @@
         <v>131</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -2006,7 +2006,7 @@
         <v>94</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>2</v>
@@ -2029,7 +2029,7 @@
         <v>132</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
@@ -2050,7 +2050,7 @@
         <v>92</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>2</v>
@@ -2073,7 +2073,7 @@
         <v>133</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
@@ -2094,7 +2094,7 @@
         <v>93</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>2</v>
@@ -2117,7 +2117,7 @@
         <v>134</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>9</v>
@@ -2138,7 +2138,7 @@
         <v>96</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>2</v>
@@ -2161,7 +2161,7 @@
         <v>135</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
@@ -2182,7 +2182,7 @@
         <v>92</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>2</v>
@@ -2205,7 +2205,7 @@
         <v>136</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
@@ -2226,7 +2226,7 @@
         <v>95</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>2</v>
@@ -2249,7 +2249,7 @@
         <v>137</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>14</v>
@@ -2270,7 +2270,7 @@
         <v>186</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J16" s="6" t="s">
         <v>185</v>
@@ -2293,7 +2293,7 @@
         <v>177</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>14</v>
@@ -2314,7 +2314,7 @@
         <v>186</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>185</v>
@@ -2337,7 +2337,7 @@
         <v>176</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>14</v>
@@ -2358,10 +2358,10 @@
         <v>181</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>43</v>
@@ -2381,7 +2381,7 @@
         <v>138</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>15</v>
@@ -2402,10 +2402,10 @@
         <v>107</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J19" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>49</v>
@@ -2425,7 +2425,7 @@
         <v>139</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>15</v>
@@ -2446,10 +2446,10 @@
         <v>107</v>
       </c>
       <c r="I20" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J20" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>49</v>
@@ -2469,7 +2469,7 @@
         <v>140</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>16</v>
@@ -2490,7 +2490,7 @@
         <v>88</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>47</v>
@@ -2513,7 +2513,7 @@
         <v>141</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>16</v>
@@ -2534,7 +2534,7 @@
         <v>88</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>48</v>
@@ -2557,7 +2557,7 @@
         <v>142</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>18</v>
@@ -2578,10 +2578,10 @@
         <v>89</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J23" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>49</v>
@@ -2601,7 +2601,7 @@
         <v>143</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>18</v>
@@ -2622,10 +2622,10 @@
         <v>91</v>
       </c>
       <c r="I24" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J24" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>49</v>
@@ -2645,7 +2645,7 @@
         <v>144</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>18</v>
@@ -2666,10 +2666,10 @@
         <v>91</v>
       </c>
       <c r="I25" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J25" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J25" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>49</v>
@@ -2689,7 +2689,7 @@
         <v>145</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>18</v>
@@ -2710,10 +2710,10 @@
         <v>91</v>
       </c>
       <c r="I26" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J26" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>49</v>
@@ -2733,7 +2733,7 @@
         <v>146</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>21</v>
@@ -2754,10 +2754,10 @@
         <v>89</v>
       </c>
       <c r="I27" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J27" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J27" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>43</v>
@@ -2777,13 +2777,13 @@
         <v>178</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>35</v>
@@ -2798,10 +2798,10 @@
         <v>89</v>
       </c>
       <c r="I28" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J28" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J28" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>43</v>
@@ -2821,13 +2821,13 @@
         <v>179</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D29" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>35</v>
@@ -2842,7 +2842,7 @@
         <v>92</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>2</v>
@@ -2865,7 +2865,7 @@
         <v>147</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>22</v>
@@ -2886,10 +2886,10 @@
         <v>89</v>
       </c>
       <c r="I30" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J30" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J30" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>43</v>
@@ -2909,7 +2909,7 @@
         <v>148</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>22</v>
@@ -2930,7 +2930,7 @@
         <v>92</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>2</v>
@@ -2953,7 +2953,7 @@
         <v>149</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>23</v>
@@ -2974,10 +2974,10 @@
         <v>107</v>
       </c>
       <c r="I32" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J32" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J32" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>43</v>
@@ -2997,7 +2997,7 @@
         <v>150</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>23</v>
@@ -3018,10 +3018,10 @@
         <v>107</v>
       </c>
       <c r="I33" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J33" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>43</v>
@@ -3041,7 +3041,7 @@
         <v>151</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>24</v>
@@ -3062,7 +3062,7 @@
         <v>107</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J34" s="6" t="s">
         <v>101</v>
@@ -3085,7 +3085,7 @@
         <v>152</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>24</v>
@@ -3106,7 +3106,7 @@
         <v>107</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>101</v>
@@ -3129,7 +3129,7 @@
         <v>153</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>24</v>
@@ -3150,7 +3150,7 @@
         <v>107</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J36" s="6" t="s">
         <v>101</v>
@@ -3173,7 +3173,7 @@
         <v>154</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>24</v>
@@ -3194,7 +3194,7 @@
         <v>107</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>101</v>
@@ -3217,7 +3217,7 @@
         <v>155</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>25</v>
@@ -3238,10 +3238,10 @@
         <v>89</v>
       </c>
       <c r="I38" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J38" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>43</v>
@@ -3261,7 +3261,7 @@
         <v>156</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>25</v>
@@ -3282,10 +3282,10 @@
         <v>91</v>
       </c>
       <c r="I39" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J39" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>43</v>
@@ -3305,7 +3305,7 @@
         <v>157</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>25</v>
@@ -3326,10 +3326,10 @@
         <v>91</v>
       </c>
       <c r="I40" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J40" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J40" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>43</v>
@@ -3349,7 +3349,7 @@
         <v>158</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>25</v>
@@ -3370,10 +3370,10 @@
         <v>91</v>
       </c>
       <c r="I41" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J41" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J41" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>43</v>
@@ -3393,7 +3393,7 @@
         <v>159</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>26</v>
@@ -3414,10 +3414,10 @@
         <v>90</v>
       </c>
       <c r="I42" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J42" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>43</v>
@@ -3437,7 +3437,7 @@
         <v>160</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>27</v>
@@ -3458,10 +3458,10 @@
         <v>90</v>
       </c>
       <c r="I43" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J43" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>43</v>
@@ -3481,7 +3481,7 @@
         <v>161</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>27</v>
@@ -3502,7 +3502,7 @@
         <v>93</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>2</v>
@@ -3525,7 +3525,7 @@
         <v>162</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>26</v>
@@ -3546,7 +3546,7 @@
         <v>93</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J45" s="6" t="s">
         <v>2</v>
@@ -3569,7 +3569,7 @@
         <v>163</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>29</v>
@@ -3590,7 +3590,7 @@
         <v>93</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>2</v>
@@ -3613,7 +3613,7 @@
         <v>164</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>29</v>
@@ -3634,7 +3634,7 @@
         <v>93</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J47" s="6" t="s">
         <v>2</v>
@@ -3657,7 +3657,7 @@
         <v>165</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>29</v>
@@ -3678,10 +3678,10 @@
         <v>108</v>
       </c>
       <c r="I48" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J48" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J48" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>43</v>
@@ -3701,7 +3701,7 @@
         <v>166</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>29</v>
@@ -3722,10 +3722,10 @@
         <v>108</v>
       </c>
       <c r="I49" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J49" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J49" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>43</v>
@@ -3745,7 +3745,7 @@
         <v>167</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>31</v>
@@ -3766,7 +3766,7 @@
         <v>112</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J50" s="6" t="s">
         <v>101</v>
@@ -3789,7 +3789,7 @@
         <v>168</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>31</v>
@@ -3810,7 +3810,7 @@
         <v>112</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J51" s="6" t="s">
         <v>101</v>
@@ -3833,7 +3833,7 @@
         <v>169</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>31</v>
@@ -3854,7 +3854,7 @@
         <v>112</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J52" s="6" t="s">
         <v>101</v>
@@ -3877,7 +3877,7 @@
         <v>170</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>31</v>
@@ -3898,7 +3898,7 @@
         <v>112</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J53" s="6" t="s">
         <v>101</v>
@@ -3921,7 +3921,7 @@
         <v>171</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>33</v>
@@ -3942,10 +3942,10 @@
         <v>90</v>
       </c>
       <c r="I54" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J54" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J54" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>60</v>
@@ -3965,7 +3965,7 @@
         <v>172</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>33</v>
@@ -3986,10 +3986,10 @@
         <v>90</v>
       </c>
       <c r="I55" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J55" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J55" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>60</v>
@@ -4009,7 +4009,7 @@
         <v>173</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>33</v>
@@ -4030,10 +4030,10 @@
         <v>90</v>
       </c>
       <c r="I56" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J56" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J56" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>60</v>
@@ -4053,7 +4053,7 @@
         <v>174</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>0</v>
@@ -4074,10 +4074,10 @@
         <v>90</v>
       </c>
       <c r="I57" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J57" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>49</v>
@@ -4097,7 +4097,7 @@
         <v>180</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>14</v>
@@ -4118,7 +4118,7 @@
         <v>183</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>188</v>
+        <v>211</v>
       </c>
       <c r="J58" s="6" t="s">
         <v>185</v>
@@ -4138,16 +4138,16 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C59" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>35</v>
@@ -4162,10 +4162,10 @@
         <v>89</v>
       </c>
       <c r="I59" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J59" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J59" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>43</v>
@@ -4182,10 +4182,10 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>102</v>
@@ -4200,16 +4200,16 @@
         <v>66</v>
       </c>
       <c r="G60" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H60" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="H60" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="I60" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J60" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J60" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>43</v>
@@ -4226,10 +4226,10 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>102</v>
@@ -4244,16 +4244,16 @@
         <v>66</v>
       </c>
       <c r="G61" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="H61" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="H61" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="I61" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J61" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J61" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K61" s="2" t="s">
         <v>43</v>
@@ -4270,10 +4270,10 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>7</v>
@@ -4288,16 +4288,16 @@
         <v>66</v>
       </c>
       <c r="G62" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H62" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="H62" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="I62" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J62" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J62" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>43</v>
@@ -4314,10 +4314,10 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>7</v>
@@ -4332,16 +4332,16 @@
         <v>66</v>
       </c>
       <c r="G63" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H63" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="H63" s="3" t="s">
-        <v>209</v>
-      </c>
       <c r="I63" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J63" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J63" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>43</v>
@@ -4358,10 +4358,10 @@
     </row>
     <row r="64" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>7</v>
@@ -4376,16 +4376,16 @@
         <v>66</v>
       </c>
       <c r="G64" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="H64" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="H64" s="7" t="s">
-        <v>205</v>
-      </c>
       <c r="I64" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J64" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J64" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K64" s="2" t="s">
         <v>43</v>
@@ -4402,10 +4402,10 @@
     </row>
     <row r="65" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>7</v>
@@ -4420,16 +4420,16 @@
         <v>66</v>
       </c>
       <c r="G65" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="H65" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="H65" s="7" t="s">
-        <v>205</v>
-      </c>
       <c r="I65" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J65" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J65" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>43</v>
@@ -4446,10 +4446,10 @@
     </row>
     <row r="66" spans="1:14" ht="153" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>5</v>
@@ -4464,16 +4464,16 @@
         <v>66</v>
       </c>
       <c r="G66" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="H66" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="H66" s="8" t="s">
-        <v>207</v>
-      </c>
       <c r="I66" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J66" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J66" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>43</v>
@@ -4493,7 +4493,7 @@
         <v>125</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>7</v>
@@ -4508,16 +4508,16 @@
         <v>66</v>
       </c>
       <c r="G67" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="H67" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="H67" s="7" t="s">
-        <v>203</v>
-      </c>
       <c r="I67" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J67" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J67" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K67" s="2" t="s">
         <v>43</v>
@@ -4537,7 +4537,7 @@
         <v>124</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>7</v>
@@ -4552,16 +4552,16 @@
         <v>66</v>
       </c>
       <c r="G68" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="H68" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="H68" s="7" t="s">
-        <v>203</v>
-      </c>
       <c r="I68" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="J68" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="J68" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="K68" s="2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
changes TX_PVLS.D/N.Routine.T to TX_PVLS.D/N.T
- changes TX_PVLS.D/N.Routine.T to TX_PVLS.D/N.T
</commit_message>
<xml_diff>
--- a/data-raw/snu_x_im_distribution_configuration/24Tto25TMap.xlsx
+++ b/data-raw/snu_x_im_distribution_configuration/24Tto25TMap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/faustolopezbao/Documents/GitHub/data-pack-commons/data-raw/snu_x_im_distribution_configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFD4009-9D77-2849-BBD5-933E1BA28A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC636A7-EC37-B740-9F36-C6D2DEA09A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="37880" yWindow="2340" windowWidth="34700" windowHeight="18800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -527,12 +527,6 @@
     <t>TX_PVLS.N.KP.T</t>
   </si>
   <si>
-    <t>TX_PVLS.D.Routine.T</t>
-  </si>
-  <si>
-    <t>TX_PVLS.N.Routine.T</t>
-  </si>
-  <si>
     <t>TX_TB.D.Already.Neg.T</t>
   </si>
   <si>
@@ -663,6 +657,12 @@
   </si>
   <si>
     <t>QCZnSIBW2BI</t>
+  </si>
+  <si>
+    <t>TX_PVLS.D.T</t>
+  </si>
+  <si>
+    <t>TX_PVLS.N.T</t>
   </si>
 </sst>
 </file>
@@ -1553,8 +1553,8 @@
   <dimension ref="A1:N68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H73" sqref="H73"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1624,7 +1624,7 @@
         <v>120</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1645,7 +1645,7 @@
         <v>97</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>2</v>
@@ -1668,7 +1668,7 @@
         <v>121</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -1689,7 +1689,7 @@
         <v>97</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>2</v>
@@ -1712,7 +1712,7 @@
         <v>122</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>6</v>
@@ -1733,10 +1733,10 @@
         <v>88</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>43</v>
@@ -1756,7 +1756,7 @@
         <v>125</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
@@ -1777,10 +1777,10 @@
         <v>118</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>49</v>
@@ -1800,7 +1800,7 @@
         <v>126</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
@@ -1821,10 +1821,10 @@
         <v>118</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>49</v>
@@ -1844,7 +1844,7 @@
         <v>127</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -1865,10 +1865,10 @@
         <v>96</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>43</v>
@@ -1888,7 +1888,7 @@
         <v>128</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
@@ -1909,10 +1909,10 @@
         <v>96</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>43</v>
@@ -1932,7 +1932,7 @@
         <v>129</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
@@ -1953,7 +1953,7 @@
         <v>93</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>2</v>
@@ -1976,7 +1976,7 @@
         <v>130</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -1997,7 +1997,7 @@
         <v>93</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>2</v>
@@ -2020,7 +2020,7 @@
         <v>131</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
@@ -2041,7 +2041,7 @@
         <v>91</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>2</v>
@@ -2064,13 +2064,13 @@
         <v>132</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>35</v>
@@ -2085,7 +2085,7 @@
         <v>92</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J12" s="6" t="s">
         <v>2</v>
@@ -2108,7 +2108,7 @@
         <v>133</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>9</v>
@@ -2129,7 +2129,7 @@
         <v>95</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J13" s="6" t="s">
         <v>2</v>
@@ -2152,7 +2152,7 @@
         <v>134</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
@@ -2173,7 +2173,7 @@
         <v>91</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>2</v>
@@ -2196,7 +2196,7 @@
         <v>135</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>13</v>
@@ -2217,7 +2217,7 @@
         <v>94</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J15" s="6" t="s">
         <v>2</v>
@@ -2240,7 +2240,7 @@
         <v>136</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>14</v>
@@ -2255,16 +2255,16 @@
         <v>65</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>43</v>
@@ -2281,10 +2281,10 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>14</v>
@@ -2299,16 +2299,16 @@
         <v>65</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>43</v>
@@ -2325,10 +2325,10 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>14</v>
@@ -2343,16 +2343,16 @@
         <v>65</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J18" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>43</v>
@@ -2372,7 +2372,7 @@
         <v>137</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>15</v>
@@ -2393,10 +2393,10 @@
         <v>106</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>49</v>
@@ -2416,7 +2416,7 @@
         <v>138</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>15</v>
@@ -2437,10 +2437,10 @@
         <v>106</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J20" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>49</v>
@@ -2460,7 +2460,7 @@
         <v>139</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>16</v>
@@ -2481,7 +2481,7 @@
         <v>87</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J21" s="6" t="s">
         <v>47</v>
@@ -2504,7 +2504,7 @@
         <v>140</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>16</v>
@@ -2525,7 +2525,7 @@
         <v>87</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J22" s="6" t="s">
         <v>48</v>
@@ -2548,7 +2548,7 @@
         <v>141</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>18</v>
@@ -2569,10 +2569,10 @@
         <v>88</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J23" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K23" s="2" t="s">
         <v>49</v>
@@ -2592,7 +2592,7 @@
         <v>142</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>18</v>
@@ -2613,10 +2613,10 @@
         <v>90</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>49</v>
@@ -2636,7 +2636,7 @@
         <v>143</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>18</v>
@@ -2657,10 +2657,10 @@
         <v>90</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>49</v>
@@ -2680,7 +2680,7 @@
         <v>144</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>18</v>
@@ -2701,10 +2701,10 @@
         <v>90</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>49</v>
@@ -2724,7 +2724,7 @@
         <v>145</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>21</v>
@@ -2745,10 +2745,10 @@
         <v>88</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J27" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>43</v>
@@ -2765,16 +2765,16 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>35</v>
@@ -2789,10 +2789,10 @@
         <v>88</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>43</v>
@@ -2809,16 +2809,16 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>35</v>
@@ -2833,7 +2833,7 @@
         <v>91</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J29" s="6" t="s">
         <v>2</v>
@@ -2856,7 +2856,7 @@
         <v>146</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>22</v>
@@ -2877,10 +2877,10 @@
         <v>88</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J30" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>43</v>
@@ -2900,7 +2900,7 @@
         <v>147</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>22</v>
@@ -2921,7 +2921,7 @@
         <v>91</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J31" s="6" t="s">
         <v>2</v>
@@ -2944,7 +2944,7 @@
         <v>148</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>23</v>
@@ -2965,10 +2965,10 @@
         <v>106</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>43</v>
@@ -2988,7 +2988,7 @@
         <v>149</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>23</v>
@@ -3009,10 +3009,10 @@
         <v>106</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>43</v>
@@ -3032,7 +3032,7 @@
         <v>150</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>24</v>
@@ -3053,7 +3053,7 @@
         <v>106</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J34" s="6" t="s">
         <v>100</v>
@@ -3076,7 +3076,7 @@
         <v>151</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>24</v>
@@ -3097,7 +3097,7 @@
         <v>106</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J35" s="6" t="s">
         <v>100</v>
@@ -3120,7 +3120,7 @@
         <v>152</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>24</v>
@@ -3141,7 +3141,7 @@
         <v>106</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J36" s="6" t="s">
         <v>100</v>
@@ -3164,7 +3164,7 @@
         <v>153</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>24</v>
@@ -3185,7 +3185,7 @@
         <v>106</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J37" s="6" t="s">
         <v>100</v>
@@ -3208,7 +3208,7 @@
         <v>154</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>25</v>
@@ -3229,10 +3229,10 @@
         <v>88</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>43</v>
@@ -3252,7 +3252,7 @@
         <v>155</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>25</v>
@@ -3273,10 +3273,10 @@
         <v>90</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>43</v>
@@ -3296,7 +3296,7 @@
         <v>156</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>25</v>
@@ -3317,10 +3317,10 @@
         <v>90</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>43</v>
@@ -3340,7 +3340,7 @@
         <v>157</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>25</v>
@@ -3361,10 +3361,10 @@
         <v>90</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>43</v>
@@ -3384,7 +3384,7 @@
         <v>158</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>26</v>
@@ -3405,10 +3405,10 @@
         <v>89</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>43</v>
@@ -3428,7 +3428,7 @@
         <v>159</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>27</v>
@@ -3449,10 +3449,10 @@
         <v>89</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>43</v>
@@ -3472,7 +3472,7 @@
         <v>160</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>27</v>
@@ -3493,7 +3493,7 @@
         <v>92</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J44" s="6" t="s">
         <v>2</v>
@@ -3516,7 +3516,7 @@
         <v>161</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>26</v>
@@ -3537,7 +3537,7 @@
         <v>92</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J45" s="6" t="s">
         <v>2</v>
@@ -3560,7 +3560,7 @@
         <v>162</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>29</v>
@@ -3581,7 +3581,7 @@
         <v>92</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J46" s="6" t="s">
         <v>2</v>
@@ -3604,7 +3604,7 @@
         <v>163</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>29</v>
@@ -3625,7 +3625,7 @@
         <v>92</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J47" s="6" t="s">
         <v>2</v>
@@ -3645,10 +3645,10 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>164</v>
+        <v>208</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>29</v>
@@ -3669,10 +3669,10 @@
         <v>107</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>43</v>
@@ -3681,7 +3681,7 @@
         <v>2</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="N48" s="2" t="s">
         <v>45</v>
@@ -3689,10 +3689,10 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>165</v>
+        <v>209</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>29</v>
@@ -3713,10 +3713,10 @@
         <v>107</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>43</v>
@@ -3725,7 +3725,7 @@
         <v>2</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="N49" s="2" t="s">
         <v>45</v>
@@ -3733,10 +3733,10 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>31</v>
@@ -3757,7 +3757,7 @@
         <v>111</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J50" s="6" t="s">
         <v>100</v>
@@ -3777,10 +3777,10 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>31</v>
@@ -3801,7 +3801,7 @@
         <v>111</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J51" s="6" t="s">
         <v>100</v>
@@ -3821,10 +3821,10 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>31</v>
@@ -3845,7 +3845,7 @@
         <v>111</v>
       </c>
       <c r="I52" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J52" s="6" t="s">
         <v>100</v>
@@ -3865,10 +3865,10 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>31</v>
@@ -3889,7 +3889,7 @@
         <v>111</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J53" s="6" t="s">
         <v>100</v>
@@ -3909,10 +3909,10 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>33</v>
@@ -3933,10 +3933,10 @@
         <v>89</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>59</v>
@@ -3953,10 +3953,10 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>33</v>
@@ -3977,10 +3977,10 @@
         <v>89</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>59</v>
@@ -3997,10 +3997,10 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>33</v>
@@ -4021,10 +4021,10 @@
         <v>89</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K56" s="2" t="s">
         <v>59</v>
@@ -4041,10 +4041,10 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>0</v>
@@ -4065,10 +4065,10 @@
         <v>89</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>49</v>
@@ -4085,10 +4085,10 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>14</v>
@@ -4103,16 +4103,16 @@
         <v>65</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H58" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="J58" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="J58" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="K58" s="4" t="s">
         <v>49</v>
@@ -4129,16 +4129,16 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>35</v>
@@ -4153,10 +4153,10 @@
         <v>88</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>43</v>
@@ -4173,10 +4173,10 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>101</v>
@@ -4191,16 +4191,16 @@
         <v>65</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>43</v>
@@ -4217,10 +4217,10 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>101</v>
@@ -4235,16 +4235,16 @@
         <v>65</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K61" s="2" t="s">
         <v>43</v>
@@ -4261,10 +4261,10 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>7</v>
@@ -4279,16 +4279,16 @@
         <v>65</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>43</v>
@@ -4305,10 +4305,10 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>7</v>
@@ -4323,16 +4323,16 @@
         <v>65</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J63" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>43</v>
@@ -4349,10 +4349,10 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>7</v>
@@ -4367,16 +4367,16 @@
         <v>65</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I64" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K64" s="2" t="s">
         <v>43</v>
@@ -4393,10 +4393,10 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>7</v>
@@ -4411,16 +4411,16 @@
         <v>65</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I65" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J65" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>43</v>
@@ -4437,16 +4437,16 @@
     </row>
     <row r="66" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>35</v>
@@ -4461,10 +4461,10 @@
         <v>89</v>
       </c>
       <c r="I66" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J66" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K66" s="2" t="s">
         <v>43</v>
@@ -4484,7 +4484,7 @@
         <v>124</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>7</v>
@@ -4499,16 +4499,16 @@
         <v>65</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J67" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K67" s="2" t="s">
         <v>43</v>
@@ -4528,7 +4528,7 @@
         <v>123</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>7</v>
@@ -4543,16 +4543,16 @@
         <v>65</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J68" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K68" s="2" t="s">
         <v>43</v>

</xml_diff>